<commit_message>
yo wtf am Idoing
</commit_message>
<xml_diff>
--- a/329_gantt_chart.xlsx
+++ b/329_gantt_chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1AF2C12-0CD2-426B-905C-9E8F4998BFAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859A8E80-94E5-4B62-8C1E-7E75AA5A27DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4005" yWindow="-180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Task 3</t>
   </si>
@@ -238,6 +238,18 @@
   </si>
   <si>
     <t>Status Report</t>
+  </si>
+  <si>
+    <t>Communincations</t>
+  </si>
+  <si>
+    <t>Nate</t>
+  </si>
+  <si>
+    <t>Budgeting</t>
+  </si>
+  <si>
+    <t>Matt &amp; Brandt</t>
   </si>
 </sst>
 </file>
@@ -887,6 +899,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -894,21 +921,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1480,7 +1492,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1524,118 +1536,118 @@
       <c r="A3" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="84" t="s">
+      <c r="B3" s="84"/>
+      <c r="C3" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="90">
+      <c r="D3" s="90"/>
+      <c r="E3" s="88">
         <v>44252</v>
       </c>
-      <c r="F3" s="90"/>
+      <c r="F3" s="88"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="85"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="85">
         <f>I5</f>
         <v>44249</v>
       </c>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="87">
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="85">
         <f>P5</f>
         <v>44256</v>
       </c>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="87">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="85">
         <f>W5</f>
         <v>44263</v>
       </c>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="87">
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87"/>
+      <c r="AD4" s="85">
         <f>AD5</f>
         <v>44270</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="87">
+      <c r="AE4" s="86"/>
+      <c r="AF4" s="86"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="86"/>
+      <c r="AJ4" s="87"/>
+      <c r="AK4" s="85">
         <f>AK5</f>
         <v>44277</v>
       </c>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="88"/>
-      <c r="AN4" s="88"/>
-      <c r="AO4" s="88"/>
-      <c r="AP4" s="88"/>
-      <c r="AQ4" s="89"/>
-      <c r="AR4" s="87">
+      <c r="AL4" s="86"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="86"/>
+      <c r="AO4" s="86"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="87"/>
+      <c r="AR4" s="85">
         <f>AR5</f>
         <v>44284</v>
       </c>
-      <c r="AS4" s="88"/>
-      <c r="AT4" s="88"/>
-      <c r="AU4" s="88"/>
-      <c r="AV4" s="88"/>
-      <c r="AW4" s="88"/>
-      <c r="AX4" s="89"/>
-      <c r="AY4" s="87">
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="86"/>
+      <c r="AU4" s="86"/>
+      <c r="AV4" s="86"/>
+      <c r="AW4" s="86"/>
+      <c r="AX4" s="87"/>
+      <c r="AY4" s="85">
         <f>AY5</f>
         <v>44291</v>
       </c>
-      <c r="AZ4" s="88"/>
-      <c r="BA4" s="88"/>
-      <c r="BB4" s="88"/>
-      <c r="BC4" s="88"/>
-      <c r="BD4" s="88"/>
-      <c r="BE4" s="89"/>
-      <c r="BF4" s="87">
+      <c r="AZ4" s="86"/>
+      <c r="BA4" s="86"/>
+      <c r="BB4" s="86"/>
+      <c r="BC4" s="86"/>
+      <c r="BD4" s="86"/>
+      <c r="BE4" s="87"/>
+      <c r="BF4" s="85">
         <f>BF5</f>
         <v>44298</v>
       </c>
-      <c r="BG4" s="88"/>
-      <c r="BH4" s="88"/>
-      <c r="BI4" s="88"/>
-      <c r="BJ4" s="88"/>
-      <c r="BK4" s="88"/>
-      <c r="BL4" s="89"/>
+      <c r="BG4" s="86"/>
+      <c r="BH4" s="86"/>
+      <c r="BI4" s="86"/>
+      <c r="BJ4" s="86"/>
+      <c r="BK4" s="86"/>
+      <c r="BL4" s="87"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44249</v>
@@ -2418,9 +2430,11 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
       <c r="B11" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="71"/>
+        <v>53</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>54</v>
+      </c>
       <c r="D11" s="22">
         <v>0.5</v>
       </c>
@@ -2497,11 +2511,13 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="58"/>
       <c r="B12" s="79" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="71"/>
+        <v>55</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>56</v>
+      </c>
       <c r="D12" s="22">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="E12" s="65">
         <f>F11</f>
@@ -4176,6 +4192,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4183,11 +4204,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">

</xml_diff>